<commit_message>
JinL - fix issues in data import and data files
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/calphi/class.xlsx
+++ b/data-transfer/transfer/data/calphi/class.xlsx
@@ -244,7 +244,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +263,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -276,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -285,6 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -574,8 +581,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -637,7 +644,7 @@
       <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -670,7 +677,7 @@
       <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -703,7 +710,7 @@
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -736,7 +743,7 @@
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -769,7 +776,7 @@
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -802,7 +809,7 @@
       <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -835,7 +842,7 @@
       <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -868,7 +875,7 @@
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -901,7 +908,7 @@
       <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -934,7 +941,7 @@
       <c r="E11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -967,7 +974,7 @@
       <c r="E12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1000,7 +1007,7 @@
       <c r="E13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -1033,7 +1040,7 @@
       <c r="E14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -1066,7 +1073,7 @@
       <c r="E15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -1099,7 +1106,7 @@
       <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -1132,7 +1139,7 @@
       <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -1165,7 +1172,7 @@
       <c r="E18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1198,7 +1205,7 @@
       <c r="E19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="11" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -1231,7 +1238,7 @@
       <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -1264,7 +1271,7 @@
       <c r="E21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -1297,7 +1304,7 @@
       <c r="E22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -1330,7 +1337,7 @@
       <c r="E23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G23" s="6" t="s">
@@ -1363,7 +1370,7 @@
       <c r="E24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -1396,7 +1403,7 @@
       <c r="E25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="6" t="s">
@@ -1429,7 +1436,7 @@
       <c r="E26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="11" t="s">
         <v>53</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -1462,7 +1469,7 @@
       <c r="E27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="11" t="s">
         <v>53</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -1495,7 +1502,7 @@
       <c r="E28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="11" t="s">
         <v>53</v>
       </c>
       <c r="G28" s="6" t="s">
@@ -1528,7 +1535,7 @@
       <c r="E29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="11" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="6" t="s">
@@ -1561,7 +1568,7 @@
       <c r="E30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G30" s="6" t="s">
@@ -1594,7 +1601,7 @@
       <c r="E31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1627,7 +1634,7 @@
       <c r="E32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G32" s="6" t="s">
@@ -1660,7 +1667,7 @@
       <c r="E33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G33" s="6" t="s">
@@ -1693,7 +1700,7 @@
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G34" s="6" t="s">
@@ -1726,7 +1733,7 @@
       <c r="E35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G35" s="6" t="s">
@@ -1759,7 +1766,7 @@
       <c r="E36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G36" s="6" t="s">
@@ -1792,7 +1799,7 @@
       <c r="E37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="11" t="s">
         <v>57</v>
       </c>
       <c r="G37" s="6" t="s">
@@ -1825,7 +1832,7 @@
       <c r="E38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="11" t="s">
         <v>57</v>
       </c>
       <c r="G38" s="6" t="s">
@@ -1858,7 +1865,7 @@
       <c r="E39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="11" t="s">
         <v>57</v>
       </c>
       <c r="G39" s="6" t="s">
@@ -1885,11 +1892,11 @@
       <c r="C40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="5"/>
+      <c r="D40" s="8"/>
       <c r="E40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="11" t="s">
         <v>57</v>
       </c>
       <c r="G40" s="6" t="s">
@@ -1922,7 +1929,7 @@
       <c r="E41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G41" s="6" t="s">
@@ -1955,7 +1962,7 @@
       <c r="E42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G42" s="6" t="s">
@@ -1988,7 +1995,7 @@
       <c r="E43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G43" s="6" t="s">
@@ -2021,7 +2028,7 @@
       <c r="E44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G44" s="6" t="s">
@@ -2054,7 +2061,7 @@
       <c r="E45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G45" s="6" t="s">
@@ -2087,7 +2094,7 @@
       <c r="E46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G46" s="6" t="s">
@@ -2120,7 +2127,7 @@
       <c r="E47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G47" s="6" t="s">
@@ -2153,7 +2160,7 @@
       <c r="E48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G48" s="6" t="s">
@@ -2186,7 +2193,7 @@
       <c r="E49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="11" t="s">
         <v>58</v>
       </c>
       <c r="G49" s="6" t="s">
@@ -2219,7 +2226,7 @@
       <c r="E50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="11" t="s">
         <v>58</v>
       </c>
       <c r="G50" s="6" t="s">
@@ -2252,7 +2259,7 @@
       <c r="E51" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G51" s="6" t="s">
@@ -2285,7 +2292,7 @@
       <c r="E52" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G52" s="6" t="s">
@@ -2318,7 +2325,7 @@
       <c r="E53" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G53" s="6" t="s">
@@ -2351,7 +2358,7 @@
       <c r="E54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="6" t="s">
@@ -2384,7 +2391,7 @@
       <c r="E55" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G55" s="6" t="s">
@@ -2417,7 +2424,7 @@
       <c r="E56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G56" s="6" t="s">
@@ -2450,7 +2457,7 @@
       <c r="E57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G57" s="6" t="s">
@@ -2483,7 +2490,7 @@
       <c r="E58" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G58" s="6" t="s">
@@ -2516,10 +2523,10 @@
       <c r="E59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H59" s="5" t="s">
@@ -2549,10 +2556,10 @@
       <c r="E60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G60" s="8" t="s">
+      <c r="G60" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H60" s="5" t="s">
@@ -2582,10 +2589,10 @@
       <c r="E61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="G61" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H61" s="5" t="s">
@@ -2615,10 +2622,10 @@
       <c r="E62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="11" t="s">
+      <c r="F62" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G62" s="8" t="s">
+      <c r="G62" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="5" t="s">
@@ -2648,10 +2655,10 @@
       <c r="E63" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G63" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H63" s="5" t="s">
@@ -2681,7 +2688,7 @@
       <c r="E64" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G64" s="6" t="s">
@@ -2714,7 +2721,7 @@
       <c r="E65" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G65" s="6" t="s">
@@ -2747,7 +2754,7 @@
       <c r="E66" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G66" s="6" t="s">
@@ -2780,10 +2787,10 @@
       <c r="E67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G67" s="8" t="s">
+      <c r="G67" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H67" s="5" t="s">
@@ -2813,10 +2820,10 @@
       <c r="E68" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F68" s="11" t="s">
+      <c r="F68" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G68" s="8" t="s">
+      <c r="G68" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H68" s="5" t="s">
@@ -2846,10 +2853,10 @@
       <c r="E69" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G69" s="8" t="s">
+      <c r="G69" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H69" s="5" t="s">
@@ -2879,10 +2886,10 @@
       <c r="E70" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G70" s="8" t="s">
+      <c r="G70" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H70" s="5" t="s">
@@ -2912,10 +2919,10 @@
       <c r="E71" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G71" s="8" t="s">
+      <c r="G71" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H71" s="5" t="s">
@@ -2945,10 +2952,10 @@
       <c r="E72" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="F72" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="G72" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H72" s="5" t="s">
@@ -2978,10 +2985,10 @@
       <c r="E73" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="F73" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G73" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H73" s="5" t="s">
@@ -3011,10 +3018,10 @@
       <c r="E74" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G74" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H74" s="5" t="s">
@@ -3044,10 +3051,10 @@
       <c r="E75" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="11" t="s">
+      <c r="F75" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G75" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H75" s="5" t="s">
@@ -3077,10 +3084,10 @@
       <c r="E76" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F76" s="11" t="s">
+      <c r="F76" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="G76" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H76" s="5" t="s">
@@ -3110,10 +3117,10 @@
       <c r="E77" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="F77" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="G77" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H77" s="5" t="s">
@@ -3143,10 +3150,10 @@
       <c r="E78" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F78" s="11" t="s">
+      <c r="F78" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="G78" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H78" s="5" t="s">
@@ -3176,10 +3183,10 @@
       <c r="E79" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="F79" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="G79" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H79" s="5" t="s">
@@ -3209,10 +3216,10 @@
       <c r="E80" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F80" s="11" t="s">
+      <c r="F80" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G80" s="9" t="s">
+      <c r="G80" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H80" s="5" t="s">
@@ -3242,10 +3249,10 @@
       <c r="E81" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F81" s="11" t="s">
+      <c r="F81" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G81" s="9" t="s">
+      <c r="G81" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H81" s="5" t="s">
@@ -3275,10 +3282,10 @@
       <c r="E82" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F82" s="11" t="s">
+      <c r="F82" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="G82" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H82" s="5" t="s">
@@ -3308,10 +3315,10 @@
       <c r="E83" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F83" s="11" t="s">
+      <c r="F83" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G83" s="9" t="s">
+      <c r="G83" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H83" s="5" t="s">
@@ -3341,10 +3348,10 @@
       <c r="E84" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F84" s="11" t="s">
+      <c r="F84" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G84" s="9" t="s">
+      <c r="G84" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H84" s="5" t="s">
@@ -3374,10 +3381,10 @@
       <c r="E85" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="F85" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G85" s="9" t="s">
+      <c r="G85" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H85" s="5" t="s">
@@ -3407,10 +3414,10 @@
       <c r="E86" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F86" s="11" t="s">
+      <c r="F86" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="G86" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H86" s="5" t="s">
@@ -3440,10 +3447,10 @@
       <c r="E87" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F87" s="11" t="s">
+      <c r="F87" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="G87" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H87" s="5" t="s">
@@ -3473,10 +3480,10 @@
       <c r="E88" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F88" s="11" t="s">
+      <c r="F88" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G88" s="9" t="s">
+      <c r="G88" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H88" s="5" t="s">
@@ -3506,10 +3513,10 @@
       <c r="E89" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="F89" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="G89" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H89" s="5" t="s">
@@ -3539,10 +3546,10 @@
       <c r="E90" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F90" s="11" t="s">
+      <c r="F90" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G90" s="9" t="s">
+      <c r="G90" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H90" s="5" t="s">
@@ -3572,10 +3579,10 @@
       <c r="E91" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="F91" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="G91" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H91" s="5" t="s">
@@ -3605,10 +3612,10 @@
       <c r="E92" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F92" s="11" t="s">
+      <c r="F92" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G92" s="9" t="s">
+      <c r="G92" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H92" s="5" t="s">
@@ -3638,10 +3645,10 @@
       <c r="E93" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="11" t="s">
+      <c r="F93" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="G93" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H93" s="5" t="s">
@@ -3671,10 +3678,10 @@
       <c r="E94" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="11" t="s">
+      <c r="F94" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G94" s="9" t="s">
+      <c r="G94" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H94" s="5" t="s">
@@ -3704,10 +3711,10 @@
       <c r="E95" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="F95" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G95" s="9" t="s">
+      <c r="G95" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H95" s="5" t="s">
@@ -3737,10 +3744,10 @@
       <c r="E96" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="11" t="s">
+      <c r="F96" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="G96" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H96" s="5" t="s">

</xml_diff>

<commit_message>
JinL - fix errors in calphi data, re-import
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/calphi/class.xlsx
+++ b/data-transfer/transfer/data/calphi/class.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="61">
   <si>
     <t>Program</t>
   </si>
@@ -244,7 +244,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,12 +263,6 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -282,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -291,7 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -581,8 +574,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F96"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -644,7 +637,7 @@
       <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -677,7 +670,7 @@
       <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -710,7 +703,7 @@
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -743,7 +736,7 @@
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -776,7 +769,7 @@
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -809,7 +802,7 @@
       <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -842,7 +835,7 @@
       <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -875,7 +868,7 @@
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -908,7 +901,7 @@
       <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -941,7 +934,7 @@
       <c r="E11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -974,7 +967,7 @@
       <c r="E12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1007,7 +1000,7 @@
       <c r="E13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -1040,7 +1033,7 @@
       <c r="E14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -1073,7 +1066,7 @@
       <c r="E15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -1106,7 +1099,7 @@
       <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -1139,7 +1132,7 @@
       <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -1172,7 +1165,7 @@
       <c r="E18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1205,7 +1198,7 @@
       <c r="E19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -1238,7 +1231,7 @@
       <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -1271,7 +1264,7 @@
       <c r="E21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -1304,7 +1297,7 @@
       <c r="E22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -1337,7 +1330,7 @@
       <c r="E23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G23" s="6" t="s">
@@ -1370,7 +1363,7 @@
       <c r="E24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -1403,7 +1396,7 @@
       <c r="E25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="6" t="s">
@@ -1436,7 +1429,7 @@
       <c r="E26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -1469,7 +1462,7 @@
       <c r="E27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -1502,7 +1495,7 @@
       <c r="E28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G28" s="6" t="s">
@@ -1535,7 +1528,7 @@
       <c r="E29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="6" t="s">
@@ -1568,7 +1561,7 @@
       <c r="E30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="10" t="s">
         <v>54</v>
       </c>
       <c r="G30" s="6" t="s">
@@ -1601,7 +1594,7 @@
       <c r="E31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1634,7 +1627,7 @@
       <c r="E32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G32" s="6" t="s">
@@ -1667,7 +1660,7 @@
       <c r="E33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="10" t="s">
         <v>54</v>
       </c>
       <c r="G33" s="6" t="s">
@@ -1700,7 +1693,7 @@
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="10" t="s">
         <v>54</v>
       </c>
       <c r="G34" s="6" t="s">
@@ -1733,7 +1726,7 @@
       <c r="E35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>56</v>
       </c>
       <c r="G35" s="6" t="s">
@@ -1766,7 +1759,7 @@
       <c r="E36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>56</v>
       </c>
       <c r="G36" s="6" t="s">
@@ -1799,7 +1792,7 @@
       <c r="E37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G37" s="6" t="s">
@@ -1832,7 +1825,7 @@
       <c r="E38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G38" s="6" t="s">
@@ -1865,7 +1858,7 @@
       <c r="E39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G39" s="6" t="s">
@@ -1892,11 +1885,13 @@
       <c r="C40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="8"/>
+      <c r="D40" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G40" s="6" t="s">
@@ -1907,7 +1902,7 @@
       </c>
       <c r="I40" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Intense 3Glider 2/3Mon,Tue,Wed,Thu16:15</v>
+        <v>Intense 3Glider 2/3Charlie O.Mon,Tue,Wed,Thu16:15</v>
       </c>
       <c r="J40" s="4">
         <v>19</v>
@@ -1929,7 +1924,7 @@
       <c r="E41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="10" t="s">
         <v>56</v>
       </c>
       <c r="G41" s="6" t="s">
@@ -1962,7 +1957,7 @@
       <c r="E42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="10" t="s">
         <v>56</v>
       </c>
       <c r="G42" s="6" t="s">
@@ -1995,7 +1990,7 @@
       <c r="E43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G43" s="6" t="s">
@@ -2028,7 +2023,7 @@
       <c r="E44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G44" s="6" t="s">
@@ -2061,7 +2056,7 @@
       <c r="E45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G45" s="6" t="s">
@@ -2094,7 +2089,7 @@
       <c r="E46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G46" s="6" t="s">
@@ -2127,7 +2122,7 @@
       <c r="E47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G47" s="6" t="s">
@@ -2160,7 +2155,7 @@
       <c r="E48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G48" s="6" t="s">
@@ -2193,7 +2188,7 @@
       <c r="E49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G49" s="6" t="s">
@@ -2226,7 +2221,7 @@
       <c r="E50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G50" s="6" t="s">
@@ -2259,7 +2254,7 @@
       <c r="E51" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G51" s="6" t="s">
@@ -2292,7 +2287,7 @@
       <c r="E52" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G52" s="6" t="s">
@@ -2325,7 +2320,7 @@
       <c r="E53" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G53" s="6" t="s">
@@ -2358,7 +2353,7 @@
       <c r="E54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="6" t="s">
@@ -2391,7 +2386,7 @@
       <c r="E55" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G55" s="6" t="s">
@@ -2424,7 +2419,7 @@
       <c r="E56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G56" s="6" t="s">
@@ -2457,7 +2452,7 @@
       <c r="E57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G57" s="6" t="s">
@@ -2490,7 +2485,7 @@
       <c r="E58" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G58" s="6" t="s">
@@ -2523,10 +2518,10 @@
       <c r="E59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="G59" s="8" t="s">
         <v>24</v>
       </c>
       <c r="H59" s="5" t="s">
@@ -2556,10 +2551,10 @@
       <c r="E60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="G60" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H60" s="5" t="s">
@@ -2589,10 +2584,10 @@
       <c r="E61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="G61" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H61" s="5" t="s">
@@ -2622,10 +2617,10 @@
       <c r="E62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="G62" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="5" t="s">
@@ -2655,10 +2650,10 @@
       <c r="E63" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H63" s="5" t="s">
@@ -2688,7 +2683,7 @@
       <c r="E64" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="11" t="s">
         <v>51</v>
       </c>
       <c r="G64" s="6" t="s">
@@ -2721,7 +2716,7 @@
       <c r="E65" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="11" t="s">
         <v>51</v>
       </c>
       <c r="G65" s="6" t="s">
@@ -2754,7 +2749,7 @@
       <c r="E66" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="11" t="s">
         <v>51</v>
       </c>
       <c r="G66" s="6" t="s">
@@ -2787,10 +2782,10 @@
       <c r="E67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G67" s="9" t="s">
+      <c r="G67" s="8" t="s">
         <v>24</v>
       </c>
       <c r="H67" s="5" t="s">
@@ -2820,10 +2815,10 @@
       <c r="E68" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G68" s="9" t="s">
+      <c r="G68" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H68" s="5" t="s">
@@ -2853,10 +2848,10 @@
       <c r="E69" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G69" s="9" t="s">
+      <c r="G69" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H69" s="5" t="s">
@@ -2886,10 +2881,10 @@
       <c r="E70" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="G70" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H70" s="5" t="s">
@@ -2919,10 +2914,10 @@
       <c r="E71" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G71" s="9" t="s">
+      <c r="G71" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H71" s="5" t="s">
@@ -2952,10 +2947,10 @@
       <c r="E72" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G72" s="10" t="s">
+      <c r="G72" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H72" s="5" t="s">
@@ -2985,10 +2980,10 @@
       <c r="E73" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G73" s="10" t="s">
+      <c r="G73" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H73" s="5" t="s">
@@ -3018,10 +3013,10 @@
       <c r="E74" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G74" s="10" t="s">
+      <c r="G74" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H74" s="5" t="s">
@@ -3051,10 +3046,10 @@
       <c r="E75" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="10" t="s">
+      <c r="G75" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H75" s="5" t="s">
@@ -3084,10 +3079,10 @@
       <c r="E76" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G76" s="10" t="s">
+      <c r="G76" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H76" s="5" t="s">
@@ -3117,10 +3112,10 @@
       <c r="E77" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G77" s="10" t="s">
+      <c r="G77" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H77" s="5" t="s">
@@ -3150,10 +3145,10 @@
       <c r="E78" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G78" s="10" t="s">
+      <c r="G78" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H78" s="5" t="s">
@@ -3183,10 +3178,10 @@
       <c r="E79" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G79" s="10" t="s">
+      <c r="G79" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H79" s="5" t="s">
@@ -3216,10 +3211,10 @@
       <c r="E80" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G80" s="10" t="s">
+      <c r="G80" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H80" s="5" t="s">
@@ -3249,10 +3244,10 @@
       <c r="E81" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F81" s="12" t="s">
+      <c r="F81" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G81" s="10" t="s">
+      <c r="G81" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H81" s="5" t="s">
@@ -3282,10 +3277,10 @@
       <c r="E82" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F82" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G82" s="10" t="s">
+      <c r="G82" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H82" s="5" t="s">
@@ -3315,10 +3310,10 @@
       <c r="E83" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F83" s="12" t="s">
+      <c r="F83" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G83" s="10" t="s">
+      <c r="G83" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H83" s="5" t="s">
@@ -3348,10 +3343,10 @@
       <c r="E84" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F84" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G84" s="10" t="s">
+      <c r="G84" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H84" s="5" t="s">
@@ -3381,10 +3376,10 @@
       <c r="E85" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F85" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G85" s="10" t="s">
+      <c r="G85" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H85" s="5" t="s">
@@ -3414,10 +3409,10 @@
       <c r="E86" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G86" s="10" t="s">
+      <c r="G86" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H86" s="5" t="s">
@@ -3447,10 +3442,10 @@
       <c r="E87" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F87" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G87" s="10" t="s">
+      <c r="G87" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H87" s="5" t="s">
@@ -3480,10 +3475,10 @@
       <c r="E88" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G88" s="10" t="s">
+      <c r="G88" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H88" s="5" t="s">
@@ -3513,10 +3508,10 @@
       <c r="E89" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F89" s="12" t="s">
+      <c r="F89" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G89" s="10" t="s">
+      <c r="G89" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H89" s="5" t="s">
@@ -3546,10 +3541,10 @@
       <c r="E90" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F90" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G90" s="10" t="s">
+      <c r="G90" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H90" s="5" t="s">
@@ -3579,10 +3574,10 @@
       <c r="E91" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="F91" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G91" s="10" t="s">
+      <c r="G91" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H91" s="5" t="s">
@@ -3612,10 +3607,10 @@
       <c r="E92" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F92" s="12" t="s">
+      <c r="F92" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G92" s="10" t="s">
+      <c r="G92" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H92" s="5" t="s">
@@ -3645,10 +3640,10 @@
       <c r="E93" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="12" t="s">
+      <c r="F93" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G93" s="10" t="s">
+      <c r="G93" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H93" s="5" t="s">
@@ -3678,10 +3673,10 @@
       <c r="E94" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F94" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G94" s="10" t="s">
+      <c r="G94" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H94" s="5" t="s">
@@ -3711,10 +3706,10 @@
       <c r="E95" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F95" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G95" s="10" t="s">
+      <c r="G95" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H95" s="5" t="s">
@@ -3744,10 +3739,10 @@
       <c r="E96" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G96" s="10" t="s">
+      <c r="G96" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H96" s="5" t="s">

</xml_diff>